<commit_message>
Minor edits to the novel impl
</commit_message>
<xml_diff>
--- a/Documents/Survey and Plan/Gantt Chart.xlsx
+++ b/Documents/Survey and Plan/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Development\GitHub\advanced-project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Development\GitHub\advanced-project\Documents\Survey and Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE5978C-F53A-49D9-A5BC-FB434E3ED47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ED2BBD-3051-4E05-AF74-11B859DE4518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{3AC3B75A-84D9-471A-A281-F2B86BB5D1A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AC3B75A-84D9-471A-A281-F2B86BB5D1A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>Implement L2P</t>
   </si>
   <si>
-    <t>Implement LNIDA</t>
-  </si>
-  <si>
     <t>Literature Implementations</t>
   </si>
   <si>
@@ -185,12 +182,6 @@
     <t>Advanced</t>
   </si>
   <si>
-    <t>Implement FearNet</t>
-  </si>
-  <si>
-    <t>Implement Mnemonics</t>
-  </si>
-  <si>
     <t>Explain Theorectical Underpinning</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>Implement Potential Solution</t>
   </si>
   <si>
-    <t>Alllocated Time for Revising Solution Design</t>
-  </si>
-  <si>
     <t>Results / Evaluation Chapter</t>
   </si>
   <si>
@@ -240,13 +228,100 @@
   </si>
   <si>
     <t>Review and Revise Presentation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mnemonics</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FearNet</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DER++</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LNIDA</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SCR</t>
+    </r>
+  </si>
+  <si>
+    <t>Allocated Time for Revising Solution Design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +345,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +371,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,32 +414,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -661,10 +755,10 @@
   <dimension ref="A1:AG53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="26" ySplit="3" topLeftCell="AA7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="26" ySplit="3" topLeftCell="AA40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM11" sqref="AM11"/>
+      <selection pane="bottomRight" activeCell="AJ52" sqref="AJ52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +940,10 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -946,10 +1040,10 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -984,7 +1078,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1023,7 +1117,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -1062,7 +1156,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1101,7 +1195,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1140,7 +1234,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1179,7 +1273,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -1217,10 +1311,10 @@
       <c r="AG10" s="7"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1240,24 +1334,24 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="7"/>
@@ -1294,9 +1388,9 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="7"/>
@@ -1336,12 +1430,12 @@
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1370,9 +1464,9 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="1"/>
@@ -1409,9 +1503,9 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="1"/>
@@ -1448,9 +1542,9 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1"/>
@@ -1487,9 +1581,9 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="1"/>
@@ -1527,19 +1621,19 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1563,15 +1657,15 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1602,9 +1696,9 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1"/>
@@ -1641,9 +1735,9 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="1"/>
@@ -1680,16 +1774,16 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1719,16 +1813,16 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1758,10 +1852,10 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1797,15 +1891,15 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="1"/>
@@ -1836,15 +1930,15 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="1"/>
@@ -1875,16 +1969,16 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -1914,16 +2008,16 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -1953,18 +2047,18 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="1"/>
@@ -1992,18 +2086,18 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
@@ -2032,25 +2126,25 @@
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="8"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -2068,10 +2162,10 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2107,15 +2201,15 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="8"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2146,15 +2240,15 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="8"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2185,15 +2279,15 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="8"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2228,22 +2322,22 @@
         <v>33</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -2261,9 +2355,9 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1"/>
@@ -2300,10 +2394,10 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2339,10 +2433,10 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2379,32 +2473,32 @@
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="11"/>
-      <c r="W41" s="11"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
@@ -2415,10 +2509,10 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2454,14 +2548,14 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -2493,10 +2587,10 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2532,10 +2626,10 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2570,11 +2664,11 @@
       <c r="AG45" s="1"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>56</v>
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2609,11 +2703,11 @@
       <c r="AG46" s="1"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>60</v>
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2648,11 +2742,11 @@
       <c r="AG47" s="1"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>61</v>
+      <c r="A48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2687,11 +2781,11 @@
       <c r="AG48" s="1"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>62</v>
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2727,8 +2821,8 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="10" t="s">
-        <v>64</v>
+      <c r="B50" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2752,22 +2846,22 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
-      <c r="Y50" s="11"/>
-      <c r="Z50" s="11"/>
-      <c r="AA50" s="11"/>
-      <c r="AB50" s="11"/>
-      <c r="AC50" s="11"/>
-      <c r="AD50" s="11"/>
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="8"/>
+      <c r="AA50" s="8"/>
+      <c r="AB50" s="8"/>
+      <c r="AC50" s="8"/>
+      <c r="AD50" s="8"/>
       <c r="AE50" s="1"/>
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2803,10 +2897,10 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>66</v>
+        <v>45</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2842,10 +2936,10 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>67</v>
+        <v>45</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>

</xml_diff>